<commit_message>
Limitato le connessioni possibili a quelle esistenti; ottimizzazione funziona, primi risultati
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/capacities_distances_v1.xlsx
+++ b/dati_casoStudioItalia/network_data/capacities_distances_v1.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Info geografiche" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Capacità di trasmissione MW" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Distanza km" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Capacità_trans_ MW_monodir" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Raw data - tr. interna 2023" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Raw data - tr. interna 2030" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Raw data - tr. interna 2035" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Raw data - tr. interna 2040" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="connection" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Info geografiche" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Capacità di trasmissione MW" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Distanza km" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Capacità_trans_ MW_monodir" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Raw data - tr. interna 2023" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Raw data - tr. interna 2030" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Raw data - tr. interna 2035" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Raw data - tr. interna 2040" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -23,13 +24,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Aptos Narrow"/>
@@ -48,7 +59,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -145,6 +156,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -154,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -168,6 +209,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -567,6 +614,289 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="8.88671875" customWidth="1" style="8" min="1" max="3"/>
+    <col width="8.88671875" customWidth="1" style="8" min="4" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="10" t="inlineStr">
+        <is>
+          <t>NORD</t>
+        </is>
+      </c>
+      <c r="C1" s="10" t="inlineStr">
+        <is>
+          <t>CNOR</t>
+        </is>
+      </c>
+      <c r="D1" s="10" t="inlineStr">
+        <is>
+          <t>CSUD</t>
+        </is>
+      </c>
+      <c r="E1" s="10" t="inlineStr">
+        <is>
+          <t>SUD</t>
+        </is>
+      </c>
+      <c r="F1" s="10" t="inlineStr">
+        <is>
+          <t>CALA</t>
+        </is>
+      </c>
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>SICI</t>
+        </is>
+      </c>
+      <c r="H1" s="10" t="inlineStr">
+        <is>
+          <t>SARD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>NORD</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>CNOR</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>CSUD</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>SUD</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>CALA</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>SICI</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>SARD</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:H8">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:H19">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -712,7 +1042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -727,44 +1057,44 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="10" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>NORD</t>
         </is>
       </c>
-      <c r="C1" s="10" t="inlineStr">
-        <is>
-          <t>CNOR</t>
-        </is>
-      </c>
-      <c r="D1" s="10" t="inlineStr">
-        <is>
-          <t>CSUD</t>
-        </is>
-      </c>
-      <c r="E1" s="10" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
+        <is>
+          <t>CNOR</t>
+        </is>
+      </c>
+      <c r="D1" s="12" t="inlineStr">
+        <is>
+          <t>CSUD</t>
+        </is>
+      </c>
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>SUD</t>
         </is>
       </c>
-      <c r="F1" s="10" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>CALA</t>
         </is>
       </c>
-      <c r="G1" s="10" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>SICI</t>
         </is>
       </c>
-      <c r="H1" s="10" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>SARD</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>NORD</t>
         </is>
@@ -792,7 +1122,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="inlineStr">
+      <c r="A3" s="12" t="inlineStr">
         <is>
           <t>CNOR</t>
         </is>
@@ -820,7 +1150,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="12" t="inlineStr">
         <is>
           <t>CSUD</t>
         </is>
@@ -848,7 +1178,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="12" t="inlineStr">
         <is>
           <t>SUD</t>
         </is>
@@ -876,7 +1206,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="12" t="inlineStr">
         <is>
           <t>CALA</t>
         </is>
@@ -904,7 +1234,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="inlineStr">
+      <c r="A7" s="12" t="inlineStr">
         <is>
           <t>SICI</t>
         </is>
@@ -932,7 +1262,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="12" t="inlineStr">
         <is>
           <t>SARD</t>
         </is>
@@ -960,39 +1290,27 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="10" t="inlineStr">
+      <c r="A9" s="12" t="inlineStr">
         <is>
           <t xml:space="preserve">SUD </t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
         <v>1100</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1247,7 +1565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1255,13 +1573,14 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="8.88671875" customWidth="1" style="8" min="1" max="16384"/>
+    <col width="8.88671875" customWidth="1" style="8" min="1" max="4"/>
+    <col width="8.88671875" customWidth="1" style="8" min="5" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1505,7 +1824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1751,7 +2070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2057,7 +2376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2393,7 +2712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Modified naming of results
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/capacities_distances_v1.xlsx
+++ b/dati_casoStudioItalia/network_data/capacities_distances_v1.xlsx
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>4300</v>
+        <v>5500</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1128,13 +1128,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3100</v>
+        <v>4700</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2900</v>
+        <v>4600</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4">
@@ -1159,19 +1159,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>2800</v>
+        <v>4500</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2400</v>
+        <v>2900</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H4" t="n">
         <v>700</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>5200</v>
+        <v>5700</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1221,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>1600</v>
+        <v>2100</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1246,19 +1246,19 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1300</v>
+        <v>2000</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
@@ -1271,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="D8" t="n">
         <v>900</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1100</v>
+        <v>1700</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Results with 15 typical days
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/capacities_distances_v1.xlsx
+++ b/dati_casoStudioItalia/network_data/capacities_distances_v1.xlsx
@@ -1103,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5500</v>
+        <v>4300</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1128,13 +1128,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4700</v>
+        <v>3100</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>4600</v>
+        <v>2900</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
@@ -1159,19 +1159,19 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>4500</v>
+        <v>2800</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2900</v>
+        <v>2400</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>700</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>5700</v>
+        <v>5200</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1221,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>2100</v>
+        <v>1600</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1246,19 +1246,19 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>2000</v>
+        <v>1300</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1271,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D8" t="n">
         <v>900</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1700</v>
+        <v>1100</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>

</xml_diff>